<commit_message>
Updated to version submitted to PLOS ONE
</commit_message>
<xml_diff>
--- a/particles_compare_final.xlsx
+++ b/particles_compare_final.xlsx
@@ -86,13 +86,13 @@
     <t xml:space="preserve">5A</t>
   </si>
   <si>
+    <t xml:space="preserve">SACLA-FR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5B</t>
+  </si>
+  <si>
     <t xml:space="preserve">48h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SACLA-FR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5B</t>
   </si>
 </sst>
 </file>
@@ -981,7 +981,7 @@
         <v>-1031.60508735868</v>
       </c>
       <c r="O12" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13">
@@ -1028,7 +1028,7 @@
         <v>41.3155999471687</v>
       </c>
       <c r="O13" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14">
@@ -1036,7 +1036,7 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" t="n">
         <v>36444</v>
@@ -1075,7 +1075,7 @@
         <v>-19.9300225690264</v>
       </c>
       <c r="O14" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15">
@@ -1122,7 +1122,7 @@
         <v>31.9371493376531</v>
       </c>
       <c r="O15" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16">
@@ -1169,7 +1169,7 @@
         <v>-8.37004702794798</v>
       </c>
       <c r="O16" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17">
@@ -1216,7 +1216,7 @@
         <v>5.1871907996919</v>
       </c>
       <c r="O17" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18">
@@ -1263,12 +1263,12 @@
         <v>-20.3403834901069</v>
       </c>
       <c r="O18" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
@@ -1294,12 +1294,12 @@
       <c r="M19"/>
       <c r="N19"/>
       <c r="O19" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
@@ -1341,15 +1341,15 @@
         <v>6.11886054688176</v>
       </c>
       <c r="O20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" t="n">
         <v>34094</v>
@@ -1388,12 +1388,12 @@
         <v>5.47379585259597</v>
       </c>
       <c r="O21" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
         <v>18</v>
@@ -1435,12 +1435,12 @@
         <v>3.57925690022921</v>
       </c>
       <c r="O22" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
         <v>16</v>
@@ -1482,7 +1482,7 @@
         <v>-16.6064890027887</v>
       </c>
       <c r="O23" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>